<commit_message>
Add logging and validate chem columns
- use python logging to store errors
- add validation methods for chem columns
- print all errors at end from log file
</commit_message>
<xml_diff>
--- a/data/upload_validation.xlsx
+++ b/data/upload_validation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="181">
   <si>
     <t xml:space="preserve">Data Source Information</t>
   </si>
@@ -453,7 +453,7 @@
     <t xml:space="preserve">SiO2</t>
   </si>
   <si>
-    <t xml:space="preserve">SiO2error</t>
+    <t xml:space="preserve">SiO2_err</t>
   </si>
   <si>
     <t xml:space="preserve">TiO2</t>
@@ -463,6 +463,12 @@
   </si>
   <si>
     <t xml:space="preserve">FeOtot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al2O3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MgO</t>
   </si>
   <si>
     <t xml:space="preserve">wt%</t>
@@ -2052,7 +2058,7 @@
   </sheetPr>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2314,7 +2320,7 @@
   </sheetPr>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2504,7 +2510,7 @@
   </sheetPr>
   <dimension ref="A1:BM6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -2825,7 +2831,7 @@
   </sheetPr>
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -3070,7 +3076,7 @@
   </sheetPr>
   <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3432,8 +3438,12 @@
   </sheetPr>
   <dimension ref="A1:BS22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="M7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="U4" activeCellId="0" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3504,8 +3514,12 @@
       <c r="R2" s="159" t="s">
         <v>136</v>
       </c>
-      <c r="S2" s="158"/>
-      <c r="T2" s="158"/>
+      <c r="S2" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="T2" s="158" t="s">
+        <v>138</v>
+      </c>
       <c r="U2" s="158"/>
       <c r="V2" s="158"/>
       <c r="W2" s="160"/>
@@ -3589,7 +3603,9 @@
       <c r="R3" s="166" t="n">
         <v>2</v>
       </c>
-      <c r="S3" s="166"/>
+      <c r="S3" s="166" t="n">
+        <v>1</v>
+      </c>
       <c r="T3" s="166"/>
       <c r="U3" s="166"/>
       <c r="V3" s="166"/>
@@ -3660,22 +3676,24 @@
         <v>53</v>
       </c>
       <c r="N4" s="171" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="O4" s="171" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="P4" s="171" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="Q4" s="171" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="R4" s="171" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="S4" s="172"/>
-      <c r="T4" s="171"/>
+      <c r="T4" s="171" t="s">
+        <v>139</v>
+      </c>
       <c r="U4" s="171"/>
       <c r="V4" s="171"/>
       <c r="W4" s="171"/>
@@ -3730,22 +3748,22 @@
     </row>
     <row r="5" s="178" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="174" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B5" s="175" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="174" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D5" s="176" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E5" s="176" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F5" s="175" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G5" s="175" t="s">
         <v>57</v>
@@ -3754,16 +3772,16 @@
         <v>58</v>
       </c>
       <c r="I5" s="176" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J5" s="175" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="K5" s="175" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L5" s="176" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="M5" s="175" t="s">
         <v>59</v>
@@ -3829,22 +3847,22 @@
     </row>
     <row r="6" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="179" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B6" s="179" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C6" s="180" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D6" s="181" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E6" s="181" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F6" s="179" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G6" s="179" t="s">
         <v>64</v>
@@ -3853,16 +3871,16 @@
         <v>65</v>
       </c>
       <c r="I6" s="181" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J6" s="179" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K6" s="179" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="L6" s="181" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="M6" s="183" t="s">
         <v>66</v>
@@ -3928,16 +3946,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N7" s="14" t="n">
         <v>47.5</v>
       </c>
       <c r="O7" s="184" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="P7" s="14" t="n">
         <v>0.61</v>
@@ -3945,10 +3963,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>160</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>158</v>
       </c>
       <c r="N8" s="14" t="n">
         <v>49.2</v>
@@ -3962,10 +3980,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N9" s="14" t="n">
         <v>48.1</v>
@@ -3976,52 +3994,52 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N10" s="14" t="n">
         <v>46</v>
       </c>
       <c r="P10" s="186" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N11" s="14" t="n">
         <v>49</v>
       </c>
       <c r="P11" s="186" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N12" s="14" t="n">
         <v>41.3</v>
       </c>
       <c r="P12" s="184" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N13" s="187" t="n">
         <v>41.667687898769</v>
@@ -4032,10 +4050,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N14" s="14" t="n">
         <v>45.4</v>
@@ -4046,10 +4064,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N15" s="14" t="n">
         <v>46</v>
@@ -4060,10 +4078,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N16" s="14" t="n">
         <v>40.8</v>
@@ -4074,10 +4092,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N17" s="14" t="n">
         <v>41</v>
@@ -4088,10 +4106,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N18" s="14" t="n">
         <v>41</v>
@@ -4102,10 +4120,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N19" s="14" t="n">
         <v>37.7</v>
@@ -4116,10 +4134,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N20" s="14" t="n">
         <v>41</v>
@@ -4130,10 +4148,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N21" s="14" t="n">
         <v>39.5</v>
@@ -4144,10 +4162,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N22" s="14" t="n">
         <v>38.3</v>
@@ -4183,7 +4201,7 @@
   </sheetPr>
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -4376,7 +4394,7 @@
       <c r="B7" s="14"/>
       <c r="C7" s="77"/>
       <c r="D7" s="14" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -4430,7 +4448,7 @@
   </sheetPr>
   <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sheet '6 Data' validation script and local notebook updated
</commit_message>
<xml_diff>
--- a/data/upload_validation.xlsx
+++ b/data/upload_validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahshi/Documents/GitHub/PyLEPR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D7C0858-A102-FA4C-9B98-39CD2F68C1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963FFA10-2753-E747-A7C1-93B56687BF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20400" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13720" yWindow="760" windowWidth="20840" windowHeight="20400" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Data Source" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="222">
   <si>
     <t>Measured Parameter</t>
   </si>
@@ -720,6 +720,36 @@
   </si>
   <si>
     <t>Run_16</t>
+  </si>
+  <si>
+    <t>wt%</t>
+  </si>
+  <si>
+    <t>&lt;abc</t>
+  </si>
+  <si>
+    <t>n.d.</t>
+  </si>
+  <si>
+    <t>≌</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>N.D</t>
+  </si>
+  <si>
+    <t>FeOtotal</t>
+  </si>
+  <si>
+    <t>FeO</t>
+  </si>
+  <si>
+    <t>Fe2O3t</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -1774,6 +1804,10 @@
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1814,10 +1848,6 @@
     <xf numFmtId="0" fontId="35" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2243,10 +2273,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="186" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="183"/>
+      <c r="B1" s="187"/>
       <c r="C1" s="96" t="s">
         <v>29</v>
       </c>
@@ -2255,7 +2285,7 @@
       <c r="A2" s="178" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="184" t="s">
+      <c r="B2" s="188" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2263,7 +2293,7 @@
       <c r="A3" s="179" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="185"/>
+      <c r="B3" s="189"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="58"/>
@@ -2515,11 +2545,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="190" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="183"/>
+      <c r="B1" s="190"/>
+      <c r="C1" s="187"/>
       <c r="D1" s="96" t="s">
         <v>29</v>
       </c>
@@ -2688,7 +2718,7 @@
       <c r="V6" s="103"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="B9" s="198" t="s">
+      <c r="B9" s="182" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2733,12 +2763,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" s="133" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="191" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
       <c r="E1" s="130" t="s">
         <v>29</v>
       </c>
@@ -3449,10 +3479,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="24" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="192" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="188"/>
+      <c r="B1" s="192"/>
       <c r="C1" s="125"/>
       <c r="D1" s="96" t="s">
         <v>29</v>
@@ -3479,8 +3509,8 @@
       <c r="Z1"/>
     </row>
     <row r="2" spans="1:26" s="24" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="189"/>
-      <c r="B2" s="190"/>
+      <c r="A2" s="193"/>
+      <c r="B2" s="194"/>
       <c r="C2" s="69"/>
       <c r="D2" s="70"/>
       <c r="E2" s="69"/>
@@ -3507,10 +3537,10 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="1:26" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="195" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="196" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="23"/>
@@ -3528,10 +3558,10 @@
       <c r="K3" s="92"/>
       <c r="L3" s="92"/>
       <c r="M3" s="23"/>
-      <c r="N3" s="193" t="s">
+      <c r="N3" s="197" t="s">
         <v>158</v>
       </c>
-      <c r="O3" s="193"/>
+      <c r="O3" s="197"/>
       <c r="P3" s="95"/>
       <c r="Q3" s="23"/>
       <c r="R3" s="93" t="s">
@@ -3754,8 +3784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BL22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3815,10 +3845,18 @@
       <c r="O2" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
+      <c r="P2" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>221</v>
+      </c>
       <c r="T2" s="9"/>
       <c r="U2" s="9"/>
       <c r="V2" s="9"/>
@@ -3878,9 +3916,7 @@
       <c r="H3" s="4">
         <v>1</v>
       </c>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
+      <c r="I3" s="4"/>
       <c r="J3" s="4">
         <v>1</v>
       </c>
@@ -3896,9 +3932,7 @@
       <c r="N3" s="4">
         <v>1</v>
       </c>
-      <c r="O3" s="4">
-        <v>1</v>
-      </c>
+      <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -3959,14 +3993,26 @@
       <c r="G4" s="129" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
+      <c r="H4" s="111" t="s">
+        <v>212</v>
+      </c>
+      <c r="I4" s="111" t="s">
+        <v>212</v>
+      </c>
       <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="111"/>
+      <c r="K4" s="111" t="s">
+        <v>212</v>
+      </c>
+      <c r="L4" s="111" t="s">
+        <v>212</v>
+      </c>
+      <c r="M4" s="111" t="s">
+        <v>212</v>
+      </c>
       <c r="N4" s="111"/>
-      <c r="O4" s="111"/>
+      <c r="O4" s="111" t="s">
+        <v>212</v>
+      </c>
       <c r="P4" s="111"/>
       <c r="Q4" s="111"/>
       <c r="R4" s="111"/>
@@ -4178,21 +4224,24 @@
       <c r="BL6" s="13"/>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="A7" s="198" t="s">
+      <c r="A7" s="182" t="s">
         <v>196</v>
       </c>
       <c r="H7" s="2">
         <v>47.5</v>
       </c>
-      <c r="I7" s="199" t="s">
+      <c r="I7" s="183" t="s">
         <v>192</v>
       </c>
       <c r="J7" s="2">
         <v>0.61</v>
       </c>
+      <c r="K7" s="2" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="A8" s="198" t="s">
+      <c r="A8" s="182" t="s">
         <v>197</v>
       </c>
       <c r="H8" s="2">
@@ -4206,62 +4255,77 @@
       </c>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="A9" s="198" t="s">
+      <c r="A9" s="182" t="s">
         <v>198</v>
       </c>
       <c r="H9" s="2">
         <v>48.1</v>
       </c>
-      <c r="J9" s="200">
+      <c r="I9" s="2">
         <v>0</v>
       </c>
+      <c r="J9" s="184">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="A10" s="198" t="s">
+      <c r="A10" s="182" t="s">
         <v>199</v>
       </c>
       <c r="H10" s="2">
         <v>46</v>
       </c>
-      <c r="J10" s="200" t="s">
+      <c r="I10" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="J10" s="184" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="A11" s="198" t="s">
+      <c r="A11" s="182" t="s">
         <v>200</v>
       </c>
       <c r="H11" s="2">
         <v>49</v>
       </c>
-      <c r="J11" s="200" t="s">
+      <c r="I11" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="J11" s="184" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="A12" s="198" t="s">
+      <c r="A12" s="182" t="s">
         <v>201</v>
       </c>
       <c r="H12" s="2">
         <v>41.3</v>
       </c>
-      <c r="J12" s="199" t="s">
+      <c r="I12" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="J12" s="183" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="A13" s="198" t="s">
+      <c r="A13" s="182" t="s">
         <v>202</v>
       </c>
-      <c r="H13" s="201">
+      <c r="H13" s="185">
         <v>41.667687898769003</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="J13" s="2">
         <v>0.7</v>
       </c>
     </row>
     <row r="14" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="A14" s="198" t="s">
+      <c r="A14" s="182" t="s">
         <v>203</v>
       </c>
       <c r="H14" s="2">
@@ -4272,7 +4336,7 @@
       </c>
     </row>
     <row r="15" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="A15" s="198" t="s">
+      <c r="A15" s="182" t="s">
         <v>204</v>
       </c>
       <c r="H15" s="2">
@@ -4283,7 +4347,7 @@
       </c>
     </row>
     <row r="16" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="A16" s="198" t="s">
+      <c r="A16" s="182" t="s">
         <v>205</v>
       </c>
       <c r="H16" s="2">
@@ -4294,7 +4358,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="198" t="s">
+      <c r="A17" s="182" t="s">
         <v>206</v>
       </c>
       <c r="H17" s="2">
@@ -4305,7 +4369,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A18" s="198" t="s">
+      <c r="A18" s="182" t="s">
         <v>207</v>
       </c>
       <c r="H18" s="2">
@@ -4316,7 +4380,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A19" s="198" t="s">
+      <c r="A19" s="182" t="s">
         <v>208</v>
       </c>
       <c r="H19" s="2">
@@ -4327,7 +4391,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A20" s="198" t="s">
+      <c r="A20" s="182" t="s">
         <v>209</v>
       </c>
       <c r="H20" s="2">
@@ -4338,7 +4402,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A21" s="198" t="s">
+      <c r="A21" s="182" t="s">
         <v>210</v>
       </c>
       <c r="H21" s="2">
@@ -4349,7 +4413,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A22" s="198" t="s">
+      <c r="A22" s="182" t="s">
         <v>211</v>
       </c>
       <c r="H22" s="2">
@@ -4409,13 +4473,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="24" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="194" t="s">
+      <c r="A1" s="198" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="195"/>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
-      <c r="E1" s="195"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
       <c r="F1" s="96" t="s">
         <v>29</v>
       </c>
@@ -4429,8 +4493,8 @@
       <c r="O1" s="25"/>
     </row>
     <row r="2" spans="1:15" s="24" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="189"/>
-      <c r="B2" s="190"/>
+      <c r="A2" s="193"/>
+      <c r="B2" s="194"/>
       <c r="C2" s="69"/>
       <c r="D2" s="70"/>
       <c r="E2" s="69"/>
@@ -4446,10 +4510,10 @@
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:15" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="195" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="196" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="23"/>
@@ -4684,8 +4748,8 @@
       <c r="AF1" s="25"/>
     </row>
     <row r="2" spans="1:32" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="189"/>
-      <c r="B2" s="190"/>
+      <c r="A2" s="193"/>
+      <c r="B2" s="194"/>
       <c r="C2" s="69"/>
       <c r="D2" s="70"/>
       <c r="E2" s="25"/>
@@ -4718,10 +4782,10 @@
       <c r="AF2" s="25"/>
     </row>
     <row r="3" spans="1:32" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="196" t="s">
+      <c r="A3" s="200" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="201" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="23"/>
@@ -4741,10 +4805,10 @@
       <c r="K3" s="94"/>
       <c r="L3" s="94"/>
       <c r="M3" s="23"/>
-      <c r="N3" s="193" t="s">
+      <c r="N3" s="197" t="s">
         <v>97</v>
       </c>
-      <c r="O3" s="193"/>
+      <c r="O3" s="197"/>
       <c r="P3" s="95"/>
       <c r="Q3" s="95"/>
       <c r="R3" s="23"/>

</xml_diff>

<commit_message>
Add back the symbol logic
</commit_message>
<xml_diff>
--- a/data/upload_validation.xlsx
+++ b/data/upload_validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahshi/Documents/GitHub/PyLEPR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963FFA10-2753-E747-A7C1-93B56687BF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7429384-8FA5-0348-AA28-E4E096EEC7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13720" yWindow="760" windowWidth="20840" windowHeight="20400" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7820" yWindow="760" windowWidth="26740" windowHeight="20380" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Data Source" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="223">
   <si>
     <t>Measured Parameter</t>
   </si>
@@ -467,9 +467,6 @@
   </si>
   <si>
     <t>grain/spot ID</t>
-  </si>
-  <si>
-    <t>enter "Liquid" for glass or mineral name from list</t>
   </si>
   <si>
     <t>Run Analytical Data</t>
@@ -750,6 +747,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>enter "Liquid" for glass or full mineral phase name from list</t>
+  </si>
+  <si>
+    <t>≤0.3</t>
   </si>
 </sst>
 </file>
@@ -2650,7 +2653,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E5" s="41" t="s">
         <v>53</v>
@@ -2719,7 +2722,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.15">
       <c r="B9" s="182" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2764,7 +2767,7 @@
   <sheetData>
     <row r="1" spans="1:64" s="133" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="191" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" s="191"/>
       <c r="C1" s="191"/>
@@ -2782,7 +2785,7 @@
       <c r="E2" s="134"/>
       <c r="F2" s="134"/>
       <c r="G2" s="128" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H2" s="135"/>
       <c r="I2" s="135"/>
@@ -2997,7 +3000,7 @@
         <v>136</v>
       </c>
       <c r="D5" s="146" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E5" s="147" t="s">
         <v>59</v>
@@ -3020,7 +3023,7 @@
         <v>137</v>
       </c>
       <c r="D6" s="148" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E6" s="148" t="s">
         <v>138</v>
@@ -3052,7 +3055,7 @@
   <dimension ref="A1:BJ6"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3067,7 +3070,7 @@
   <sheetData>
     <row r="1" spans="1:62" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="160" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" s="160"/>
       <c r="C1" s="162"/>
@@ -3081,7 +3084,7 @@
       <c r="C2" s="105"/>
       <c r="D2" s="105"/>
       <c r="E2" s="128" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -3360,7 +3363,7 @@
         <v>120</v>
       </c>
       <c r="B6" s="181" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C6" s="148" t="s">
         <v>138</v>
@@ -3480,7 +3483,7 @@
   <sheetData>
     <row r="1" spans="1:26" s="24" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="192" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" s="192"/>
       <c r="C1" s="125"/>
@@ -3538,14 +3541,14 @@
     </row>
     <row r="3" spans="1:26" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="195" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="196" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="87" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E3" s="87"/>
       <c r="F3" s="87"/>
@@ -3553,25 +3556,25 @@
       <c r="H3" s="88"/>
       <c r="I3" s="23"/>
       <c r="J3" s="92" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K3" s="92"/>
       <c r="L3" s="92"/>
       <c r="M3" s="23"/>
       <c r="N3" s="197" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O3" s="197"/>
       <c r="P3" s="95"/>
       <c r="Q3" s="23"/>
       <c r="R3" s="93" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S3" s="93"/>
       <c r="T3" s="93"/>
       <c r="U3" s="82"/>
       <c r="V3" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W3" s="34"/>
       <c r="X3" s="34"/>
@@ -3580,10 +3583,10 @@
     </row>
     <row r="4" spans="1:26" s="18" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="118" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="163" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="64" t="s">
@@ -3596,40 +3599,40 @@
         <v>9</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H4" s="66" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="172" t="s">
+        <v>170</v>
+      </c>
+      <c r="K4" s="77" t="s">
+        <v>172</v>
+      </c>
+      <c r="L4" s="77" t="s">
         <v>171</v>
-      </c>
-      <c r="K4" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="L4" s="77" t="s">
-        <v>172</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="85" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O4" s="85" t="s">
+        <v>161</v>
+      </c>
+      <c r="P4" s="85" t="s">
         <v>162</v>
-      </c>
-      <c r="P4" s="85" t="s">
-        <v>163</v>
       </c>
       <c r="Q4" s="17"/>
       <c r="R4" s="78" t="s">
         <v>132</v>
       </c>
       <c r="S4" s="78" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T4" s="78" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="U4" s="16"/>
       <c r="V4" s="79"/>
@@ -3640,23 +3643,23 @@
     </row>
     <row r="5" spans="1:26" s="30" customFormat="1" ht="52" x14ac:dyDescent="0.2">
       <c r="A5" s="167" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="167" t="s">
         <v>150</v>
-      </c>
-      <c r="B5" s="167" t="s">
-        <v>151</v>
       </c>
       <c r="C5" s="164"/>
       <c r="D5" s="165" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="165" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F5" s="173" t="s">
         <v>25</v>
       </c>
       <c r="G5" s="165" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H5" s="40" t="s">
         <v>19</v>
@@ -3670,7 +3673,7 @@
         <v>128</v>
       </c>
       <c r="O5" s="169" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P5" s="169" t="s">
         <v>130</v>
@@ -3683,7 +3686,7 @@
         <v>129</v>
       </c>
       <c r="T5" s="173" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U5" s="17"/>
       <c r="V5" s="79"/>
@@ -3784,8 +3787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BL22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3800,7 +3803,7 @@
   <sheetData>
     <row r="1" spans="1:64" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="160" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" s="161"/>
       <c r="C1" s="162"/>
@@ -3822,40 +3825,40 @@
         <v>54</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>191</v>
-      </c>
       <c r="P2" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>221</v>
       </c>
       <c r="T2" s="9"/>
       <c r="U2" s="9"/>
@@ -3994,24 +3997,24 @@
         <v>56</v>
       </c>
       <c r="H4" s="111" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I4" s="111" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J4" s="111"/>
       <c r="K4" s="111" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L4" s="111" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M4" s="111" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N4" s="111"/>
       <c r="O4" s="111" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P4" s="111"/>
       <c r="Q4" s="111"/>
@@ -4143,12 +4146,12 @@
       <c r="BK5" s="2"/>
       <c r="BL5" s="2"/>
     </row>
-    <row r="6" spans="1:64" ht="52" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:64" ht="56" x14ac:dyDescent="0.15">
       <c r="A6" s="49" t="s">
         <v>120</v>
       </c>
       <c r="B6" s="159" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="C6" s="114" t="s">
         <v>63</v>
@@ -4225,24 +4228,24 @@
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.15">
       <c r="A7" s="182" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H7" s="2">
         <v>47.5</v>
       </c>
       <c r="I7" s="183" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J7" s="2">
         <v>0.61</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.15">
       <c r="A8" s="182" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H8" s="2">
         <v>49.2</v>
@@ -4256,7 +4259,7 @@
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.15">
       <c r="A9" s="182" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H9" s="2">
         <v>48.1</v>
@@ -4270,55 +4273,55 @@
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.15">
       <c r="A10" s="182" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H10" s="2">
         <v>46</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J10" s="184" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.15">
       <c r="A11" s="182" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H11" s="2">
         <v>49</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J11" s="184" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.15">
       <c r="A12" s="182" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H12" s="2">
         <v>41.3</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J12" s="183" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:64" x14ac:dyDescent="0.15">
       <c r="A13" s="182" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H13" s="185">
         <v>41.667687898769003</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J13" s="2">
         <v>0.7</v>
@@ -4326,18 +4329,21 @@
     </row>
     <row r="14" spans="1:64" x14ac:dyDescent="0.15">
       <c r="A14" s="182" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H14" s="2">
         <v>45.4</v>
       </c>
+      <c r="I14" s="2" t="s">
+        <v>222</v>
+      </c>
       <c r="J14" s="2">
         <v>0.9</v>
       </c>
     </row>
     <row r="15" spans="1:64" x14ac:dyDescent="0.15">
       <c r="A15" s="182" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H15" s="2">
         <v>46</v>
@@ -4348,7 +4354,7 @@
     </row>
     <row r="16" spans="1:64" x14ac:dyDescent="0.15">
       <c r="A16" s="182" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H16" s="2">
         <v>40.799999999999997</v>
@@ -4359,7 +4365,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="182" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H17" s="2">
         <v>41</v>
@@ -4370,7 +4376,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="182" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H18" s="2">
         <v>41</v>
@@ -4381,7 +4387,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="182" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H19" s="2">
         <v>37.700000000000003</v>
@@ -4392,7 +4398,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="182" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H20" s="2">
         <v>41</v>
@@ -4403,7 +4409,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="182" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H21" s="2">
         <v>39.5</v>
@@ -4414,7 +4420,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="182" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H22" s="2">
         <v>38.299999999999997</v>
@@ -4437,7 +4443,7 @@
     <hyperlink ref="G2" r:id="rId1" xr:uid="{4D420096-6EDD-6E47-8444-EE1A1DB5AA58}"/>
     <hyperlink ref="G4" r:id="rId2" xr:uid="{3B498634-FC0E-0C4F-8272-3634D08CBC1E}"/>
     <hyperlink ref="G3" location="'7 Primary Method Metadata'!A5" display="METHOD CODE [more info]:" xr:uid="{C912465B-86E5-7E48-BC13-34397909EE63}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{6BD747FE-E8D1-E548-B9F3-F2AD61BC2E17}"/>
+    <hyperlink ref="B6" r:id="rId3" display="enter &quot;Liquid&quot; for glass or mineral name from list" xr:uid="{6BD747FE-E8D1-E548-B9F3-F2AD61BC2E17}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4579,10 +4585,10 @@
     </row>
     <row r="5" spans="1:15" s="30" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A5" s="119" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="119" t="s">
         <v>147</v>
-      </c>
-      <c r="B5" s="119" t="s">
-        <v>148</v>
       </c>
       <c r="C5" s="67"/>
       <c r="D5" s="127" t="s">
@@ -4825,7 +4831,7 @@
       <c r="AA3" s="95"/>
       <c r="AB3" s="82"/>
       <c r="AC3" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AD3" s="34"/>
       <c r="AE3" s="34"/>
@@ -4911,10 +4917,10 @@
     </row>
     <row r="5" spans="1:32" s="75" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A5" s="119" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="119" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C5" s="81"/>
       <c r="D5" s="51"/>

</xml_diff>

<commit_message>
Fix validation for symbols, alter import method
</commit_message>
<xml_diff>
--- a/data/upload_validation.xlsx
+++ b/data/upload_validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahshi/Documents/GitHub/PyLEPR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3747192D-F98F-4640-B93C-C9D166AE7420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDBC7C5-C6A5-4A42-987B-2CED2ADD3402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23620" windowHeight="20380" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12300" yWindow="760" windowWidth="23620" windowHeight="20380" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Data Source" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="253">
   <si>
     <t>Measured Parameter</t>
   </si>
@@ -457,9 +457,6 @@
     <t>FeO*</t>
   </si>
   <si>
-    <t>FeOtot</t>
-  </si>
-  <si>
     <t>Al2O3</t>
   </si>
   <si>
@@ -538,12 +535,6 @@
     <t>≌</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>N.D</t>
-  </si>
-  <si>
     <t>FeO</t>
   </si>
   <si>
@@ -574,9 +565,6 @@
     <t>liquid</t>
   </si>
   <si>
-    <t>cpx</t>
-  </si>
-  <si>
     <t>opx</t>
   </si>
   <si>
@@ -595,15 +583,9 @@
     <t>liq;ol;opx</t>
   </si>
   <si>
-    <t>liq, o, op</t>
-  </si>
-  <si>
     <t>liquid, olivine, opx</t>
   </si>
   <si>
-    <t>liquid, orthopyroxene</t>
-  </si>
-  <si>
     <t>Al2O3_err</t>
   </si>
   <si>
@@ -611,15 +593,6 @@
   </si>
   <si>
     <t>FeO*_err</t>
-  </si>
-  <si>
-    <t>FeOtot_err</t>
-  </si>
-  <si>
-    <t>Fe2O3total</t>
-  </si>
-  <si>
-    <t>Fe2O3total_err</t>
   </si>
   <si>
     <t>Must match an experiment on the EXPERIMENTS tab column A</t>
@@ -773,9 +746,6 @@
     <t>liq</t>
   </si>
   <si>
-    <t>vol%</t>
-  </si>
-  <si>
     <t>EMPA</t>
   </si>
   <si>
@@ -857,10 +827,22 @@
     <t>orthopyroxene</t>
   </si>
   <si>
-    <t>&lt;1</t>
-  </si>
-  <si>
-    <t>&gt;3</t>
+    <t>opx_err</t>
+  </si>
+  <si>
+    <t>liq_err</t>
+  </si>
+  <si>
+    <t>liquid, opx</t>
+  </si>
+  <si>
+    <t>FeO_err</t>
+  </si>
+  <si>
+    <t>Fe2O3</t>
+  </si>
+  <si>
+    <t>Total_err</t>
   </si>
 </sst>
 </file>
@@ -1970,6 +1952,187 @@
     <xf numFmtId="49" fontId="47" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="15" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="15" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="16" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2010,189 +2173,10 @@
     <xf numFmtId="0" fontId="35" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="15" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="15" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="16" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2618,10 +2602,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="238" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="178"/>
+      <c r="B1" s="239"/>
       <c r="C1" s="88" t="s">
         <v>25</v>
       </c>
@@ -2630,7 +2614,7 @@
       <c r="A2" s="150" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="240" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2638,7 +2622,7 @@
       <c r="A3" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="180"/>
+      <c r="B3" s="241"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="52"/>
@@ -2868,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="H1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2890,11 +2874,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="181" t="s">
+      <c r="A1" s="242" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="178"/>
+      <c r="B1" s="242"/>
+      <c r="C1" s="239"/>
       <c r="D1" s="88" t="s">
         <v>25</v>
       </c>
@@ -2941,19 +2925,19 @@
         <v>92</v>
       </c>
       <c r="B4" s="131" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C4" s="131" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D4" s="132" t="s">
         <v>107</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="G4" s="34" t="s">
         <v>98</v>
@@ -2965,13 +2949,13 @@
         <v>95</v>
       </c>
       <c r="J4" s="134" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="K4" s="134" t="s">
         <v>97</v>
       </c>
       <c r="L4" s="160" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="M4" s="160"/>
       <c r="N4" s="160"/>
@@ -2986,22 +2970,22 @@
     </row>
     <row r="5" spans="1:22" s="26" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="36" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C5" s="166" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D5" s="38" t="s">
         <v>125</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="G5" s="165" t="s">
         <v>110</v>
@@ -3019,7 +3003,7 @@
         <v>109</v>
       </c>
       <c r="L5" s="133" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="M5" s="133"/>
       <c r="N5" s="39"/>
@@ -3064,19 +3048,22 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C7" s="2">
         <v>1234</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>223</v>
+      </c>
       <c r="E7" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
@@ -3088,30 +3075,30 @@
         <v>1</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C8" s="2">
         <v>1234</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="G8" s="2">
         <v>2</v>
@@ -3126,30 +3113,30 @@
         <v>1</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C9" s="2">
         <v>1234</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="G9" s="2">
         <v>3</v>
@@ -3164,30 +3151,30 @@
         <v>1</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C10" s="2">
         <v>1234</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="G10" s="2">
         <v>4</v>
@@ -3202,10 +3189,10 @@
         <v>1</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3234,10 +3221,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB839336-BA14-2045-A8D0-963F349663C6}">
-  <dimension ref="A1:BL13"/>
+  <dimension ref="A1:BM13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3249,19 +3236,19 @@
     <col min="8" max="16384" width="10.6640625" style="121"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="115" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="182" t="s">
+    <row r="1" spans="1:65" s="115" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A1" s="243" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
       <c r="E1" s="112" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="114"/>
     </row>
-    <row r="2" spans="1:64" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="94"/>
       <c r="B2" s="116"/>
       <c r="C2" s="116"/>
@@ -3284,15 +3271,19 @@
         <v>133</v>
       </c>
       <c r="L2" s="117" t="s">
+        <v>135</v>
+      </c>
+      <c r="M2" s="117" t="s">
+        <v>178</v>
+      </c>
+      <c r="N2" s="117" t="s">
         <v>136</v>
       </c>
-      <c r="M2" s="117" t="s">
-        <v>137</v>
-      </c>
-      <c r="N2" s="117"/>
-      <c r="O2" s="117"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="119"/>
+      <c r="O2" s="117" t="s">
+        <v>179</v>
+      </c>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="118"/>
       <c r="R2" s="119"/>
       <c r="S2" s="119"/>
       <c r="T2" s="119"/>
@@ -3322,7 +3313,7 @@
       <c r="AR2" s="119"/>
       <c r="AS2" s="119"/>
       <c r="AT2" s="119"/>
-      <c r="AU2" s="120"/>
+      <c r="AU2" s="119"/>
       <c r="AV2" s="120"/>
       <c r="AW2" s="120"/>
       <c r="AX2" s="120"/>
@@ -3340,8 +3331,9 @@
       <c r="BJ2" s="120"/>
       <c r="BK2" s="120"/>
       <c r="BL2" s="120"/>
-    </row>
-    <row r="3" spans="1:64" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="BM2" s="120"/>
+    </row>
+    <row r="3" spans="1:65" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="122"/>
       <c r="B3" s="113"/>
       <c r="C3" s="113"/>
@@ -3367,10 +3359,14 @@
         <v>2</v>
       </c>
       <c r="M3" s="123">
+        <v>2</v>
+      </c>
+      <c r="N3" s="123">
         <v>3</v>
       </c>
-      <c r="N3" s="123"/>
-      <c r="O3" s="123"/>
+      <c r="O3" s="123">
+        <v>3</v>
+      </c>
       <c r="P3" s="123"/>
       <c r="Q3" s="123"/>
       <c r="R3" s="123"/>
@@ -3401,7 +3397,7 @@
       <c r="AQ3" s="123"/>
       <c r="AR3" s="123"/>
       <c r="AS3" s="123"/>
-      <c r="AT3" s="124"/>
+      <c r="AT3" s="123"/>
       <c r="AU3" s="124"/>
       <c r="AV3" s="124"/>
       <c r="AW3" s="124"/>
@@ -3420,8 +3416,9 @@
       <c r="BJ3" s="124"/>
       <c r="BK3" s="124"/>
       <c r="BL3" s="124"/>
-    </row>
-    <row r="4" spans="1:64" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="BM3" s="124"/>
+    </row>
+    <row r="4" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="125"/>
       <c r="B4" s="115"/>
       <c r="C4" s="115"/>
@@ -3432,23 +3429,27 @@
         <v>51</v>
       </c>
       <c r="H4" s="126" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I4" s="126" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J4" s="126" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K4" s="126"/>
       <c r="L4" s="126" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M4" s="126" t="s">
-        <v>158</v>
-      </c>
-      <c r="N4" s="126"/>
-      <c r="O4" s="126"/>
+        <v>157</v>
+      </c>
+      <c r="N4" s="126" t="s">
+        <v>157</v>
+      </c>
+      <c r="O4" s="126" t="s">
+        <v>157</v>
+      </c>
       <c r="P4" s="126"/>
       <c r="Q4" s="126"/>
       <c r="R4" s="126"/>
@@ -3479,7 +3480,7 @@
       <c r="AQ4" s="126"/>
       <c r="AR4" s="126"/>
       <c r="AS4" s="126"/>
-      <c r="AT4" s="127"/>
+      <c r="AT4" s="126"/>
       <c r="AU4" s="127"/>
       <c r="AV4" s="127"/>
       <c r="AW4" s="127"/>
@@ -3498,33 +3499,34 @@
       <c r="BJ4" s="127"/>
       <c r="BK4" s="127"/>
       <c r="BL4" s="127"/>
-    </row>
-    <row r="5" spans="1:64" ht="51" x14ac:dyDescent="0.15">
-      <c r="A5" s="193" t="s">
+      <c r="BM4" s="127"/>
+    </row>
+    <row r="5" spans="1:65" ht="51" x14ac:dyDescent="0.15">
+      <c r="A5" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="194" t="s">
+      <c r="B5" s="178" t="s">
         <v>99</v>
       </c>
       <c r="C5" s="169" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D5" s="169" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E5" s="169" t="s">
-        <v>193</v>
-      </c>
-      <c r="F5" s="195" t="s">
-        <v>232</v>
-      </c>
-      <c r="G5" s="196" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="6" spans="1:64" s="128" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="197" t="s">
-        <v>226</v>
+        <v>184</v>
+      </c>
+      <c r="F5" s="179" t="s">
+        <v>222</v>
+      </c>
+      <c r="G5" s="180" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65" s="128" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="181" t="s">
+        <v>217</v>
       </c>
       <c r="B6" s="172" t="s">
         <v>93</v>
@@ -3533,24 +3535,27 @@
         <v>108</v>
       </c>
       <c r="D6" s="172" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E6" s="172" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="F6" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="198" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.15">
+      <c r="G6" s="182" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:65" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="121" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B7" s="121" t="s">
-        <v>242</v>
+        <v>232</v>
+      </c>
+      <c r="F7" s="254" t="s">
+        <v>233</v>
       </c>
       <c r="H7" s="121">
         <v>48</v>
@@ -3567,11 +3572,11 @@
       <c r="L7" s="121">
         <v>14</v>
       </c>
-      <c r="M7" s="121">
+      <c r="N7" s="121">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.15">
       <c r="D13" s="163"/>
     </row>
   </sheetData>
@@ -3593,8 +3598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9301B48-277D-8246-980E-7536882E3373}">
   <dimension ref="A1:BJ14"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3626,13 +3631,17 @@
         <v>129</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+        <v>219</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>248</v>
+      </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
@@ -3701,8 +3710,12 @@
       <c r="G3" s="4">
         <v>4</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="4">
+        <v>4</v>
+      </c>
+      <c r="I3" s="4">
+        <v>4</v>
+      </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -3766,13 +3779,17 @@
         <v>51</v>
       </c>
       <c r="F4" s="101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G4" s="101" t="s">
-        <v>229</v>
-      </c>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
+        <v>157</v>
+      </c>
+      <c r="H4" s="101" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="101" t="s">
+        <v>157</v>
+      </c>
       <c r="J4" s="101"/>
       <c r="K4" s="101"/>
       <c r="L4" s="101"/>
@@ -3832,16 +3849,16 @@
         <v>92</v>
       </c>
       <c r="B5" s="168" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C5" s="169" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D5" s="164" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="E5" s="168" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -3903,19 +3920,19 @@
     </row>
     <row r="6" spans="1:62" ht="65" x14ac:dyDescent="0.15">
       <c r="A6" s="170" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B6" s="171" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C6" s="172" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D6" s="173" t="s">
         <v>52</v>
       </c>
       <c r="E6" s="173" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -3977,13 +3994,13 @@
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A7" s="153" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="F7" s="2">
         <v>47.5</v>
@@ -3994,16 +4011,16 @@
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A8" s="153" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>257</v>
+        <v>233</v>
+      </c>
+      <c r="F8" s="2">
+        <v>47.5</v>
       </c>
       <c r="G8" s="2">
         <v>49.2</v>
@@ -4011,13 +4028,13 @@
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A9" s="153" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="F9" s="2">
         <v>48.1</v>
@@ -4028,30 +4045,30 @@
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A10" s="153" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="F10" s="2">
         <v>46</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>258</v>
+      <c r="G10" s="2">
+        <v>47.5</v>
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A11" s="153" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="F11" s="2">
         <v>49</v>
@@ -4062,10 +4079,10 @@
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A12" s="153" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F12" s="2">
         <v>41.3</v>
@@ -4076,10 +4093,10 @@
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A13" s="153" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F13" s="157">
         <v>41.66</v>
@@ -4092,10 +4109,10 @@
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A14" s="153" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>183</v>
+        <v>249</v>
       </c>
       <c r="F14" s="2">
         <v>45.4</v>
@@ -4120,7 +4137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAD3D8F-E56C-A042-B18B-973E8E62E26F}">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -4152,10 +4169,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="244" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="183"/>
+      <c r="B1" s="244"/>
       <c r="C1" s="109"/>
       <c r="D1" s="88" t="s">
         <v>25</v>
@@ -4182,8 +4199,8 @@
       <c r="Z1"/>
     </row>
     <row r="2" spans="1:26" s="21" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="184"/>
-      <c r="B2" s="185"/>
+      <c r="A2" s="245"/>
+      <c r="B2" s="246"/>
       <c r="C2" s="63"/>
       <c r="D2" s="64"/>
       <c r="E2" s="63"/>
@@ -4210,10 +4227,10 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="1:26" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="186" t="s">
+      <c r="A3" s="247" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="187" t="s">
+      <c r="B3" s="248" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="20"/>
@@ -4231,10 +4248,10 @@
       <c r="K3" s="84"/>
       <c r="L3" s="84"/>
       <c r="M3" s="20"/>
-      <c r="N3" s="188" t="s">
+      <c r="N3" s="249" t="s">
         <v>116</v>
       </c>
-      <c r="O3" s="188"/>
+      <c r="O3" s="249"/>
       <c r="P3" s="87"/>
       <c r="Q3" s="20"/>
       <c r="R3" s="85" t="s">
@@ -4256,67 +4273,67 @@
         <v>115</v>
       </c>
       <c r="B4" s="158" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="58" t="s">
         <v>98</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="F4" s="58" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="59" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="H4" s="60" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="144" t="s">
         <v>123</v>
       </c>
       <c r="K4" s="71" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="L4" s="71" t="s">
-        <v>249</v>
-      </c>
-      <c r="M4" s="204"/>
+        <v>239</v>
+      </c>
+      <c r="M4" s="186"/>
       <c r="N4" s="77" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="O4" s="77" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="P4" s="77" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="Q4" s="15"/>
       <c r="R4" s="72" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="S4" s="72" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="T4" s="72" t="s">
-        <v>255</v>
-      </c>
-      <c r="U4" s="204"/>
+        <v>245</v>
+      </c>
+      <c r="U4" s="186"/>
       <c r="V4" s="73"/>
       <c r="W4" s="73"/>
       <c r="X4" s="149"/>
       <c r="Y4" s="149"/>
-      <c r="Z4" s="205"/>
-    </row>
-    <row r="5" spans="1:26" s="208" customFormat="1" ht="52" x14ac:dyDescent="0.15">
-      <c r="A5" s="206" t="s">
-        <v>213</v>
-      </c>
-      <c r="B5" s="206" t="s">
-        <v>214</v>
+      <c r="Z4" s="187"/>
+    </row>
+    <row r="5" spans="1:26" s="190" customFormat="1" ht="52" x14ac:dyDescent="0.15">
+      <c r="A5" s="188" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="188" t="s">
+        <v>205</v>
       </c>
       <c r="C5" s="138"/>
       <c r="D5" s="139" t="s">
@@ -4329,7 +4346,7 @@
         <v>22</v>
       </c>
       <c r="G5" s="139" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="H5" s="37" t="s">
         <v>17</v>
@@ -4338,7 +4355,7 @@
       <c r="J5" s="146"/>
       <c r="K5" s="71"/>
       <c r="L5" s="71"/>
-      <c r="M5" s="207"/>
+      <c r="M5" s="189"/>
       <c r="N5" s="141" t="s">
         <v>104</v>
       </c>
@@ -4455,10 +4472,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BP22"/>
+  <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4471,7 +4488,7 @@
     <col min="8" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:62" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="135" t="s">
         <v>112</v>
       </c>
@@ -4484,7 +4501,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="100"/>
     </row>
-    <row r="2" spans="1:68" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:62" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="94"/>
       <c r="B2" s="95"/>
       <c r="C2" s="6"/>
@@ -4507,41 +4524,31 @@
         <v>133</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="M2" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>186</v>
-      </c>
       <c r="O2" s="7" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>187</v>
+        <v>251</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>165</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
       <c r="X2" s="9"/>
       <c r="Y2" s="9"/>
       <c r="Z2" s="9"/>
@@ -4563,12 +4570,12 @@
       <c r="AP2" s="9"/>
       <c r="AQ2" s="9"/>
       <c r="AR2" s="9"/>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9"/>
-      <c r="AU2" s="9"/>
-      <c r="AV2" s="9"/>
-      <c r="AW2" s="9"/>
-      <c r="AX2" s="9"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
       <c r="AY2" s="1"/>
       <c r="AZ2" s="1"/>
       <c r="BA2" s="1"/>
@@ -4581,14 +4588,8 @@
       <c r="BH2" s="1"/>
       <c r="BI2" s="1"/>
       <c r="BJ2" s="1"/>
-      <c r="BK2" s="1"/>
-      <c r="BL2" s="1"/>
-      <c r="BM2" s="1"/>
-      <c r="BN2" s="1"/>
-      <c r="BO2" s="1"/>
-      <c r="BP2" s="1"/>
-    </row>
-    <row r="3" spans="1:68" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:62" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="96"/>
       <c r="B3" s="97"/>
       <c r="C3" s="99"/>
@@ -4626,26 +4627,16 @@
         <v>1</v>
       </c>
       <c r="Q3" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R3" s="4">
-        <v>1</v>
-      </c>
-      <c r="S3" s="4">
-        <v>1</v>
-      </c>
-      <c r="T3" s="4">
-        <v>1</v>
-      </c>
-      <c r="U3" s="4">
-        <v>1</v>
-      </c>
-      <c r="V3" s="4">
-        <v>1</v>
-      </c>
-      <c r="W3" s="4">
         <v>5</v>
       </c>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
@@ -4666,12 +4657,12 @@
       <c r="AO3" s="4"/>
       <c r="AP3" s="4"/>
       <c r="AQ3" s="4"/>
-      <c r="AR3" s="4"/>
-      <c r="AS3" s="4"/>
-      <c r="AT3" s="4"/>
-      <c r="AU3" s="4"/>
-      <c r="AV3" s="4"/>
-      <c r="AW3" s="4"/>
+      <c r="AR3" s="5"/>
+      <c r="AS3" s="5"/>
+      <c r="AT3" s="5"/>
+      <c r="AU3" s="5"/>
+      <c r="AV3" s="5"/>
+      <c r="AW3" s="5"/>
       <c r="AX3" s="5"/>
       <c r="AY3" s="5"/>
       <c r="AZ3" s="5"/>
@@ -4685,71 +4676,54 @@
       <c r="BH3" s="5"/>
       <c r="BI3" s="5"/>
       <c r="BJ3" s="5"/>
-      <c r="BK3" s="5"/>
-      <c r="BL3" s="5"/>
-      <c r="BM3" s="5"/>
-      <c r="BN3" s="5"/>
-      <c r="BO3" s="5"/>
-      <c r="BP3" s="5"/>
-    </row>
-    <row r="4" spans="1:68" ht="14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:62" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="96"/>
-      <c r="B4" s="199"/>
-      <c r="C4" s="200"/>
-      <c r="D4" s="201"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="201"/>
+      <c r="B4" s="97"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
       <c r="G4" s="175" t="s">
         <v>51</v>
       </c>
       <c r="H4" s="101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I4" s="101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J4" s="101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K4" s="101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L4" s="101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M4" s="101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N4" s="101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O4" s="101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P4" s="101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q4" s="101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R4" s="101" t="s">
-        <v>158</v>
-      </c>
-      <c r="S4" s="101" t="s">
-        <v>158</v>
-      </c>
-      <c r="T4" s="101" t="s">
-        <v>158</v>
-      </c>
-      <c r="U4" s="101" t="s">
-        <v>158</v>
-      </c>
-      <c r="V4" s="101" t="s">
-        <v>158</v>
-      </c>
-      <c r="W4" s="101" t="s">
-        <v>158</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="S4" s="101"/>
+      <c r="T4" s="101"/>
+      <c r="U4" s="101"/>
+      <c r="V4" s="101"/>
+      <c r="W4" s="101"/>
       <c r="X4" s="101"/>
       <c r="Y4" s="101"/>
       <c r="Z4" s="101"/>
@@ -4770,12 +4744,12 @@
       <c r="AO4" s="101"/>
       <c r="AP4" s="101"/>
       <c r="AQ4" s="101"/>
-      <c r="AR4" s="101"/>
-      <c r="AS4" s="101"/>
-      <c r="AT4" s="101"/>
-      <c r="AU4" s="101"/>
-      <c r="AV4" s="101"/>
-      <c r="AW4" s="101"/>
+      <c r="AR4" s="102"/>
+      <c r="AS4" s="102"/>
+      <c r="AT4" s="102"/>
+      <c r="AU4" s="102"/>
+      <c r="AV4" s="102"/>
+      <c r="AW4" s="102"/>
       <c r="AX4" s="102"/>
       <c r="AY4" s="102"/>
       <c r="AZ4" s="102"/>
@@ -4789,34 +4763,28 @@
       <c r="BH4" s="102"/>
       <c r="BI4" s="102"/>
       <c r="BJ4" s="102"/>
-      <c r="BK4" s="102"/>
-      <c r="BL4" s="102"/>
-      <c r="BM4" s="102"/>
-      <c r="BN4" s="102"/>
-      <c r="BO4" s="102"/>
-      <c r="BP4" s="102"/>
-    </row>
-    <row r="5" spans="1:68" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:62" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="167" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="202" t="s">
+      <c r="B5" s="184" t="s">
         <v>111</v>
       </c>
       <c r="C5" s="168" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D5" s="168" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="E5" s="168" t="s">
-        <v>193</v>
-      </c>
-      <c r="F5" s="195" t="s">
-        <v>232</v>
-      </c>
-      <c r="G5" s="196" t="s">
-        <v>194</v>
+        <v>184</v>
+      </c>
+      <c r="F5" s="179" t="s">
+        <v>222</v>
+      </c>
+      <c r="G5" s="180" t="s">
+        <v>185</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -4873,19 +4841,13 @@
       <c r="BH5" s="2"/>
       <c r="BI5" s="2"/>
       <c r="BJ5" s="2"/>
-      <c r="BK5" s="2"/>
-      <c r="BL5" s="2"/>
-      <c r="BM5" s="2"/>
-      <c r="BN5" s="2"/>
-      <c r="BO5" s="2"/>
-      <c r="BP5" s="2"/>
-    </row>
-    <row r="6" spans="1:68" ht="56" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:62" ht="56" x14ac:dyDescent="0.15">
       <c r="A6" s="170" t="s">
-        <v>190</v>
-      </c>
-      <c r="B6" s="203" t="s">
-        <v>210</v>
+        <v>181</v>
+      </c>
+      <c r="B6" s="185" t="s">
+        <v>201</v>
       </c>
       <c r="C6" s="173" t="s">
         <v>53</v>
@@ -4894,13 +4856,13 @@
         <v>29</v>
       </c>
       <c r="E6" s="173" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="F6" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="198" t="s">
-        <v>212</v>
+      <c r="G6" s="182" t="s">
+        <v>203</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -4957,39 +4919,35 @@
       <c r="BH6" s="12"/>
       <c r="BI6" s="12"/>
       <c r="BJ6" s="12"/>
-      <c r="BK6" s="12"/>
-      <c r="BL6" s="12"/>
-      <c r="BM6" s="12"/>
-      <c r="BN6" s="12"/>
-      <c r="BO6" s="12"/>
-      <c r="BP6" s="12"/>
-    </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A7" s="153" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F7" s="209"/>
+        <v>168</v>
+      </c>
+      <c r="F7" s="191"/>
       <c r="H7" s="2">
         <v>47.5</v>
       </c>
       <c r="I7" s="154" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J7" s="2">
         <v>0.61</v>
       </c>
       <c r="K7" s="156" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:62" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="153" t="s">
-        <v>143</v>
-      </c>
-      <c r="F8" s="209"/>
+        <v>142</v>
+      </c>
+      <c r="F8" s="191" t="s">
+        <v>233</v>
+      </c>
       <c r="H8" s="2">
         <v>49.2</v>
       </c>
@@ -5000,257 +4958,281 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="9" spans="1:68" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:62" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="153" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F9" s="209" t="s">
-        <v>243</v>
+        <v>169</v>
+      </c>
+      <c r="F9" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H9" s="2">
         <v>48.1</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="156">
         <v>0</v>
       </c>
       <c r="J9" s="2">
         <v>0.42</v>
       </c>
     </row>
-    <row r="10" spans="1:68" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:62" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="153" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F10" s="209" t="s">
-        <v>243</v>
+        <v>165</v>
+      </c>
+      <c r="F10" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H10" s="2">
         <v>46</v>
       </c>
       <c r="I10" s="156" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J10" s="155" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:68" ht="14" x14ac:dyDescent="0.15">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:62" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="153" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F11" s="209" t="s">
-        <v>243</v>
+        <v>166</v>
+      </c>
+      <c r="F11" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H11" s="2">
         <v>49</v>
       </c>
-      <c r="I11" s="156" t="s">
-        <v>163</v>
+      <c r="I11" s="255">
+        <v>0.3</v>
       </c>
       <c r="J11" s="155" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:68" ht="14" x14ac:dyDescent="0.15">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:62" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="153" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F12" s="209" t="s">
-        <v>243</v>
+        <v>167</v>
+      </c>
+      <c r="F12" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H12" s="2">
         <v>41.3</v>
       </c>
-      <c r="I12" s="156" t="s">
-        <v>161</v>
+      <c r="I12" s="255">
+        <v>0.3</v>
       </c>
       <c r="J12" s="154" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:68" ht="14" x14ac:dyDescent="0.15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:62" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="153" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F13" s="209" t="s">
-        <v>243</v>
+        <v>170</v>
+      </c>
+      <c r="F13" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H13" s="157">
         <v>41.66</v>
       </c>
-      <c r="I13" s="156" t="s">
-        <v>162</v>
+      <c r="I13" s="255">
+        <v>0.3</v>
       </c>
       <c r="J13" s="2">
         <v>0.7</v>
       </c>
     </row>
-    <row r="14" spans="1:68" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:62" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="153" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F14" s="209" t="s">
-        <v>243</v>
+        <v>170</v>
+      </c>
+      <c r="F14" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H14" s="2">
         <v>45.4</v>
       </c>
       <c r="I14" s="156" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J14" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="1:68" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:62" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="153" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F15" s="209" t="s">
-        <v>243</v>
+        <v>168</v>
+      </c>
+      <c r="F15" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H15" s="2">
         <v>46</v>
       </c>
+      <c r="I15" s="255" t="s">
+        <v>160</v>
+      </c>
       <c r="J15" s="2">
         <v>0.74</v>
       </c>
     </row>
-    <row r="16" spans="1:68" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:62" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="153" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="F16" s="209" t="s">
-        <v>243</v>
+        <v>246</v>
+      </c>
+      <c r="F16" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H16" s="2">
         <v>40.799999999999997</v>
       </c>
+      <c r="I16" s="255">
+        <v>0.3</v>
+      </c>
       <c r="J16" s="2">
         <v>0.64</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="153" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F17" s="209" t="s">
-        <v>243</v>
+        <v>168</v>
+      </c>
+      <c r="F17" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H17" s="2">
         <v>41</v>
       </c>
+      <c r="I17" s="255">
+        <v>0.3</v>
+      </c>
       <c r="J17" s="2">
         <v>0.7</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="153" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F18" s="209" t="s">
-        <v>243</v>
+        <v>164</v>
+      </c>
+      <c r="F18" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H18" s="2">
         <v>41</v>
       </c>
+      <c r="I18" s="255">
+        <v>0.3</v>
+      </c>
       <c r="J18" s="2">
         <v>0.7</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="153" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F19" s="209" t="s">
-        <v>243</v>
+        <v>169</v>
+      </c>
+      <c r="F19" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H19" s="2">
         <v>37.700000000000003</v>
       </c>
+      <c r="I19" s="255">
+        <v>0.3</v>
+      </c>
       <c r="J19" s="2">
         <v>0.63</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="153" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F20" s="209" t="s">
-        <v>243</v>
+        <v>165</v>
+      </c>
+      <c r="F20" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H20" s="2">
         <v>41</v>
       </c>
+      <c r="I20" s="255">
+        <v>0.3</v>
+      </c>
       <c r="J20" s="2">
         <v>0.8</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="153" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F21" s="209" t="s">
-        <v>243</v>
+        <v>166</v>
+      </c>
+      <c r="F21" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H21" s="2">
         <v>39.5</v>
       </c>
+      <c r="I21" s="255">
+        <v>0.3</v>
+      </c>
       <c r="J21" s="2">
         <v>0.71</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="153" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F22" s="209" t="s">
-        <v>243</v>
+        <v>167</v>
+      </c>
+      <c r="F22" s="191" t="s">
+        <v>233</v>
       </c>
       <c r="H22" s="2">
         <v>38.299999999999997</v>
+      </c>
+      <c r="I22" s="255">
+        <v>0.3</v>
       </c>
       <c r="J22" s="2">
         <v>0.7</v>
@@ -5306,13 +5288,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="250" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
+      <c r="B1" s="251"/>
+      <c r="C1" s="251"/>
+      <c r="D1" s="251"/>
+      <c r="E1" s="251"/>
       <c r="F1" s="88" t="s">
         <v>25</v>
       </c>
@@ -5326,8 +5308,8 @@
       <c r="O1" s="22"/>
     </row>
     <row r="2" spans="1:15" s="21" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="184"/>
-      <c r="B2" s="185"/>
+      <c r="A2" s="245"/>
+      <c r="B2" s="246"/>
       <c r="C2" s="63"/>
       <c r="D2" s="64"/>
       <c r="E2" s="63"/>
@@ -5343,10 +5325,10 @@
       <c r="O2" s="22"/>
     </row>
     <row r="3" spans="1:15" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="186" t="s">
+      <c r="A3" s="247" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="187" t="s">
+      <c r="B3" s="248" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="20"/>
@@ -5368,105 +5350,105 @@
       <c r="O3" s="81"/>
     </row>
     <row r="4" spans="1:15" s="159" customFormat="1" ht="68" x14ac:dyDescent="0.15">
-      <c r="A4" s="231" t="s">
+      <c r="A4" s="213" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="252" t="s">
+      <c r="B4" s="234" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="235"/>
-      <c r="D4" s="254" t="s">
+      <c r="C4" s="217"/>
+      <c r="D4" s="236" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="253" t="s">
+      <c r="E4" s="235" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="247" t="s">
+      <c r="F4" s="229" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="253" t="s">
+      <c r="G4" s="235" t="s">
+        <v>186</v>
+      </c>
+      <c r="H4" s="237" t="s">
+        <v>187</v>
+      </c>
+      <c r="I4" s="217"/>
+      <c r="J4" s="202" t="s">
+        <v>188</v>
+      </c>
+      <c r="K4" s="230" t="s">
+        <v>189</v>
+      </c>
+      <c r="L4" s="202" t="s">
+        <v>190</v>
+      </c>
+      <c r="M4" s="230" t="s">
+        <v>191</v>
+      </c>
+      <c r="N4" s="202" t="s">
+        <v>192</v>
+      </c>
+      <c r="O4" s="218" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="27" customFormat="1" ht="65" x14ac:dyDescent="0.15">
+      <c r="A5" s="214" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="188" t="s">
         <v>195</v>
       </c>
-      <c r="H4" s="255" t="s">
-        <v>196</v>
-      </c>
-      <c r="I4" s="235"/>
-      <c r="J4" s="220" t="s">
-        <v>197</v>
-      </c>
-      <c r="K4" s="248" t="s">
-        <v>198</v>
-      </c>
-      <c r="L4" s="220" t="s">
-        <v>199</v>
-      </c>
-      <c r="M4" s="248" t="s">
-        <v>200</v>
-      </c>
-      <c r="N4" s="220" t="s">
-        <v>201</v>
-      </c>
-      <c r="O4" s="236" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="27" customFormat="1" ht="65" x14ac:dyDescent="0.15">
-      <c r="A5" s="232" t="s">
-        <v>203</v>
-      </c>
-      <c r="B5" s="206" t="s">
-        <v>204</v>
-      </c>
-      <c r="C5" s="244"/>
-      <c r="D5" s="246" t="s">
+      <c r="C5" s="226"/>
+      <c r="D5" s="228" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="139" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="245" t="s">
+      <c r="F5" s="227" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="139" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="H5" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="244"/>
+      <c r="I5" s="226"/>
       <c r="J5" s="140" t="s">
         <v>89</v>
       </c>
-      <c r="K5" s="211"/>
+      <c r="K5" s="193"/>
       <c r="L5" s="140" t="s">
         <v>55</v>
       </c>
-      <c r="M5" s="211" t="s">
-        <v>206</v>
+      <c r="M5" s="193" t="s">
+        <v>197</v>
       </c>
       <c r="N5" s="140" t="s">
         <v>55</v>
       </c>
-      <c r="O5" s="237" t="s">
-        <v>207</v>
+      <c r="O5" s="219" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="224"/>
+      <c r="A6" s="206"/>
       <c r="B6" s="103"/>
-      <c r="C6" s="249"/>
+      <c r="C6" s="231"/>
       <c r="D6" s="111"/>
       <c r="E6" s="47"/>
-      <c r="F6" s="250"/>
+      <c r="F6" s="232"/>
       <c r="G6" s="47"/>
       <c r="H6" s="62"/>
-      <c r="I6" s="249"/>
+      <c r="I6" s="231"/>
       <c r="J6" s="48"/>
-      <c r="K6" s="226"/>
+      <c r="K6" s="208"/>
       <c r="L6" s="48"/>
-      <c r="M6" s="226"/>
+      <c r="M6" s="208"/>
       <c r="N6" s="48"/>
-      <c r="O6" s="251"/>
+      <c r="O6" s="233"/>
     </row>
     <row r="7" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="104">
@@ -5475,7 +5457,7 @@
       <c r="B7" s="2"/>
       <c r="C7" s="56"/>
       <c r="D7" s="2" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -5493,7 +5475,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
@@ -5534,7 +5516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AF10"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
@@ -5603,8 +5585,8 @@
       <c r="AF1" s="22"/>
     </row>
     <row r="2" spans="1:32" s="21" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="184"/>
-      <c r="B2" s="185"/>
+      <c r="A2" s="245"/>
+      <c r="B2" s="246"/>
       <c r="C2" s="63"/>
       <c r="D2" s="64"/>
       <c r="E2" s="22"/>
@@ -5637,10 +5619,10 @@
       <c r="AF2" s="22"/>
     </row>
     <row r="3" spans="1:32" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="252" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="253" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="20"/>
@@ -5660,10 +5642,10 @@
       <c r="K3" s="86"/>
       <c r="L3" s="86"/>
       <c r="M3" s="20"/>
-      <c r="N3" s="188" t="s">
+      <c r="N3" s="249" t="s">
         <v>84</v>
       </c>
-      <c r="O3" s="188"/>
+      <c r="O3" s="249"/>
       <c r="P3" s="87"/>
       <c r="Q3" s="87"/>
       <c r="R3" s="20"/>
@@ -5687,101 +5669,101 @@
       <c r="AF3" s="31"/>
     </row>
     <row r="4" spans="1:32" s="69" customFormat="1" ht="51" x14ac:dyDescent="0.15">
-      <c r="A4" s="231" t="s">
+      <c r="A4" s="213" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="217" t="s">
+      <c r="B4" s="199" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="235"/>
-      <c r="D4" s="218" t="s">
+      <c r="C4" s="217"/>
+      <c r="D4" s="200" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="218" t="s">
+      <c r="E4" s="200" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="235"/>
-      <c r="G4" s="219" t="s">
+      <c r="F4" s="217"/>
+      <c r="G4" s="201" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="219" t="s">
+      <c r="H4" s="201" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="235"/>
-      <c r="J4" s="220" t="s">
+      <c r="I4" s="217"/>
+      <c r="J4" s="202" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="220" t="s">
+      <c r="K4" s="202" t="s">
         <v>75</v>
       </c>
-      <c r="L4" s="220" t="s">
+      <c r="L4" s="202" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="233"/>
-      <c r="N4" s="238" t="s">
+      <c r="M4" s="215"/>
+      <c r="N4" s="220" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="221" t="s">
+      <c r="O4" s="203" t="s">
         <v>79</v>
       </c>
-      <c r="P4" s="240" t="s">
+      <c r="P4" s="222" t="s">
         <v>72</v>
       </c>
-      <c r="Q4" s="221" t="s">
+      <c r="Q4" s="203" t="s">
         <v>73</v>
       </c>
-      <c r="R4" s="235"/>
-      <c r="S4" s="221" t="s">
+      <c r="R4" s="217"/>
+      <c r="S4" s="203" t="s">
         <v>63</v>
       </c>
-      <c r="T4" s="240" t="s">
+      <c r="T4" s="222" t="s">
         <v>64</v>
       </c>
-      <c r="U4" s="221" t="s">
+      <c r="U4" s="203" t="s">
         <v>65</v>
       </c>
-      <c r="V4" s="240" t="s">
+      <c r="V4" s="222" t="s">
         <v>66</v>
       </c>
-      <c r="W4" s="221" t="s">
+      <c r="W4" s="203" t="s">
         <v>67</v>
       </c>
-      <c r="X4" s="240" t="s">
+      <c r="X4" s="222" t="s">
         <v>68</v>
       </c>
-      <c r="Y4" s="221" t="s">
+      <c r="Y4" s="203" t="s">
         <v>69</v>
       </c>
-      <c r="Z4" s="240" t="s">
+      <c r="Z4" s="222" t="s">
         <v>70</v>
       </c>
-      <c r="AA4" s="221" t="s">
+      <c r="AA4" s="203" t="s">
         <v>71</v>
       </c>
-      <c r="AB4" s="235"/>
-      <c r="AC4" s="222"/>
-      <c r="AD4" s="241"/>
-      <c r="AE4" s="223"/>
-      <c r="AF4" s="242"/>
+      <c r="AB4" s="217"/>
+      <c r="AC4" s="204"/>
+      <c r="AD4" s="223"/>
+      <c r="AE4" s="205"/>
+      <c r="AF4" s="224"/>
     </row>
     <row r="5" spans="1:32" s="69" customFormat="1" ht="65" x14ac:dyDescent="0.2">
-      <c r="A5" s="232" t="s">
-        <v>208</v>
-      </c>
-      <c r="B5" s="206" t="s">
-        <v>209</v>
-      </c>
-      <c r="C5" s="210"/>
+      <c r="A5" s="214" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="188" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="192"/>
       <c r="D5" s="70"/>
-      <c r="E5" s="215" t="s">
+      <c r="E5" s="197" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="210"/>
+      <c r="F5" s="192"/>
       <c r="G5" s="71"/>
-      <c r="H5" s="216" t="s">
+      <c r="H5" s="198" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="210"/>
+      <c r="I5" s="192"/>
       <c r="J5" s="140" t="s">
         <v>74</v>
       </c>
@@ -5791,68 +5773,68 @@
       <c r="L5" s="140" t="s">
         <v>77</v>
       </c>
-      <c r="M5" s="234"/>
-      <c r="N5" s="239" t="s">
+      <c r="M5" s="216"/>
+      <c r="N5" s="221" t="s">
         <v>82</v>
       </c>
       <c r="O5" s="141" t="s">
         <v>81</v>
       </c>
-      <c r="P5" s="212" t="s">
+      <c r="P5" s="194" t="s">
         <v>80</v>
       </c>
       <c r="Q5" s="141" t="s">
         <v>83</v>
       </c>
-      <c r="R5" s="210"/>
+      <c r="R5" s="192"/>
       <c r="S5" s="77"/>
-      <c r="T5" s="213"/>
+      <c r="T5" s="195"/>
       <c r="U5" s="77"/>
-      <c r="V5" s="213"/>
+      <c r="V5" s="195"/>
       <c r="W5" s="77"/>
-      <c r="X5" s="213"/>
+      <c r="X5" s="195"/>
       <c r="Y5" s="77"/>
-      <c r="Z5" s="213"/>
+      <c r="Z5" s="195"/>
       <c r="AA5" s="77"/>
-      <c r="AB5" s="210"/>
+      <c r="AB5" s="192"/>
       <c r="AC5" s="73"/>
-      <c r="AD5" s="214"/>
+      <c r="AD5" s="196"/>
       <c r="AE5" s="74"/>
-      <c r="AF5" s="243"/>
+      <c r="AF5" s="225"/>
     </row>
     <row r="6" spans="1:32" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="224"/>
+      <c r="A6" s="206"/>
       <c r="B6" s="103"/>
-      <c r="C6" s="225"/>
+      <c r="C6" s="207"/>
       <c r="D6" s="45"/>
       <c r="E6" s="105"/>
-      <c r="F6" s="225"/>
+      <c r="F6" s="207"/>
       <c r="G6" s="46"/>
       <c r="H6" s="106"/>
-      <c r="I6" s="225"/>
+      <c r="I6" s="207"/>
       <c r="J6" s="48"/>
       <c r="K6" s="48"/>
       <c r="L6" s="48"/>
-      <c r="M6" s="225"/>
-      <c r="N6" s="227"/>
+      <c r="M6" s="207"/>
+      <c r="N6" s="209"/>
       <c r="O6" s="107"/>
-      <c r="P6" s="227"/>
+      <c r="P6" s="209"/>
       <c r="Q6" s="107"/>
-      <c r="R6" s="225"/>
+      <c r="R6" s="207"/>
       <c r="S6" s="78"/>
-      <c r="T6" s="228"/>
+      <c r="T6" s="210"/>
       <c r="U6" s="78"/>
-      <c r="V6" s="228"/>
+      <c r="V6" s="210"/>
       <c r="W6" s="78"/>
-      <c r="X6" s="228"/>
+      <c r="X6" s="210"/>
       <c r="Y6" s="78"/>
-      <c r="Z6" s="228"/>
+      <c r="Z6" s="210"/>
       <c r="AA6" s="78"/>
-      <c r="AB6" s="225"/>
+      <c r="AB6" s="207"/>
       <c r="AC6" s="18"/>
-      <c r="AD6" s="229"/>
+      <c r="AD6" s="211"/>
       <c r="AE6" s="19"/>
-      <c r="AF6" s="230"/>
+      <c r="AF6" s="212"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A7" s="104">

</xml_diff>

<commit_message>
Add validation functions for checking fO2, analytical techniques, units
</commit_message>
<xml_diff>
--- a/data/upload_validation.xlsx
+++ b/data/upload_validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahshi/Documents/GitHub/PyLEPR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDBC7C5-C6A5-4A42-987B-2CED2ADD3402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED34896C-2628-6D41-84F9-5D38D822CFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12300" yWindow="760" windowWidth="23620" windowHeight="20380" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10940" yWindow="760" windowWidth="23620" windowHeight="20380" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Data Source" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="256">
   <si>
     <t>Measured Parameter</t>
   </si>
@@ -749,9 +749,6 @@
     <t>EMPA</t>
   </si>
   <si>
-    <t>Point Counting</t>
-  </si>
-  <si>
     <t>CALCULATED AVERAGE</t>
   </si>
   <si>
@@ -833,9 +830,6 @@
     <t>liq_err</t>
   </si>
   <si>
-    <t>liquid, opx</t>
-  </si>
-  <si>
     <t>FeO_err</t>
   </si>
   <si>
@@ -843,6 +837,21 @@
   </si>
   <si>
     <t>Total_err</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>EMP</t>
+  </si>
+  <si>
+    <t>point_count</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>wt.%</t>
   </si>
 </sst>
 </file>
@@ -2133,6 +2142,9 @@
     <xf numFmtId="49" fontId="11" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2173,10 +2185,7 @@
     <xf numFmtId="0" fontId="35" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2602,10 +2611,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="239" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="239"/>
+      <c r="B1" s="240"/>
       <c r="C1" s="88" t="s">
         <v>25</v>
       </c>
@@ -2614,7 +2623,7 @@
       <c r="A2" s="150" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="240" t="s">
+      <c r="B2" s="241" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2622,7 +2631,7 @@
       <c r="A3" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="241"/>
+      <c r="B3" s="242"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="52"/>
@@ -2852,8 +2861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2874,11 +2883,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="242" t="s">
+      <c r="A1" s="243" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="239"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="240"/>
       <c r="D1" s="88" t="s">
         <v>25</v>
       </c>
@@ -2925,19 +2934,19 @@
         <v>92</v>
       </c>
       <c r="B4" s="131" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C4" s="131" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D4" s="132" t="s">
         <v>107</v>
       </c>
       <c r="E4" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="F4" s="35" t="s">
         <v>228</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>229</v>
       </c>
       <c r="G4" s="34" t="s">
         <v>98</v>
@@ -3051,19 +3060,19 @@
         <v>141</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C7" s="2">
         <v>1234</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
@@ -3074,11 +3083,11 @@
       <c r="J7" s="2">
         <v>1</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="255">
+        <v>10000</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.15">
@@ -3086,19 +3095,19 @@
         <v>142</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C8" s="2">
         <v>1234</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="G8" s="2">
         <v>2</v>
@@ -3113,10 +3122,10 @@
         <v>1</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.15">
@@ -3124,19 +3133,19 @@
         <v>143</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C9" s="2">
         <v>1234</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="G9" s="2">
         <v>3</v>
@@ -3151,10 +3160,10 @@
         <v>1</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.15">
@@ -3162,19 +3171,19 @@
         <v>144</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C10" s="2">
         <v>1234</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="G10" s="2">
         <v>4</v>
@@ -3189,10 +3198,10 @@
         <v>1</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3223,7 +3232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB839336-BA14-2045-A8D0-963F349663C6}">
   <dimension ref="A1:BM13"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -3237,12 +3246,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" s="115" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="243" t="s">
+      <c r="A1" s="244" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
+      <c r="B1" s="244"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
       <c r="E1" s="112" t="s">
         <v>25</v>
       </c>
@@ -3518,7 +3527,7 @@
         <v>184</v>
       </c>
       <c r="F5" s="179" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G5" s="180" t="s">
         <v>185</v>
@@ -3549,13 +3558,13 @@
     </row>
     <row r="7" spans="1:65" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="121" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B7" s="121" t="s">
+        <v>231</v>
+      </c>
+      <c r="F7" s="238" t="s">
         <v>232</v>
-      </c>
-      <c r="F7" s="254" t="s">
-        <v>233</v>
       </c>
       <c r="H7" s="121">
         <v>48</v>
@@ -3637,10 +3646,10 @@
         <v>219</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>248</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -3855,7 +3864,7 @@
         <v>184</v>
       </c>
       <c r="D5" s="164" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E5" s="168" t="s">
         <v>185</v>
@@ -4000,7 +4009,7 @@
         <v>172</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F7" s="2">
         <v>47.5</v>
@@ -4017,7 +4026,7 @@
         <v>173</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F8" s="2">
         <v>47.5</v>
@@ -4034,7 +4043,7 @@
         <v>174</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F9" s="2">
         <v>48.1</v>
@@ -4051,7 +4060,7 @@
         <v>175</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F10" s="2">
         <v>46</v>
@@ -4068,7 +4077,7 @@
         <v>176</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F11" s="2">
         <v>49</v>
@@ -4084,6 +4093,9 @@
       <c r="B12" s="2" t="s">
         <v>174</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="F12" s="2">
         <v>41.3</v>
       </c>
@@ -4098,6 +4110,9 @@
       <c r="B13" s="2" t="s">
         <v>177</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="F13" s="157">
         <v>41.66</v>
       </c>
@@ -4112,7 +4127,7 @@
         <v>148</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>249</v>
+        <v>219</v>
       </c>
       <c r="F14" s="2">
         <v>45.4</v>
@@ -4169,10 +4184,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="244" t="s">
+      <c r="A1" s="245" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="244"/>
+      <c r="B1" s="245"/>
       <c r="C1" s="109"/>
       <c r="D1" s="88" t="s">
         <v>25</v>
@@ -4199,8 +4214,8 @@
       <c r="Z1"/>
     </row>
     <row r="2" spans="1:26" s="21" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="245"/>
-      <c r="B2" s="246"/>
+      <c r="A2" s="246"/>
+      <c r="B2" s="247"/>
       <c r="C2" s="63"/>
       <c r="D2" s="64"/>
       <c r="E2" s="63"/>
@@ -4227,10 +4242,10 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="1:26" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="247" t="s">
+      <c r="A3" s="248" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="248" t="s">
+      <c r="B3" s="249" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="20"/>
@@ -4248,10 +4263,10 @@
       <c r="K3" s="84"/>
       <c r="L3" s="84"/>
       <c r="M3" s="20"/>
-      <c r="N3" s="249" t="s">
+      <c r="N3" s="250" t="s">
         <v>116</v>
       </c>
-      <c r="O3" s="249"/>
+      <c r="O3" s="250"/>
       <c r="P3" s="87"/>
       <c r="Q3" s="20"/>
       <c r="R3" s="85" t="s">
@@ -4273,53 +4288,53 @@
         <v>115</v>
       </c>
       <c r="B4" s="158" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="58" t="s">
         <v>98</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F4" s="58" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="H4" s="60" t="s">
         <v>236</v>
-      </c>
-      <c r="H4" s="60" t="s">
-        <v>237</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="144" t="s">
         <v>123</v>
       </c>
       <c r="K4" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="L4" s="71" t="s">
         <v>238</v>
-      </c>
-      <c r="L4" s="71" t="s">
-        <v>239</v>
       </c>
       <c r="M4" s="186"/>
       <c r="N4" s="77" t="s">
+        <v>239</v>
+      </c>
+      <c r="O4" s="77" t="s">
         <v>240</v>
       </c>
-      <c r="O4" s="77" t="s">
+      <c r="P4" s="77" t="s">
         <v>241</v>
-      </c>
-      <c r="P4" s="77" t="s">
-        <v>242</v>
       </c>
       <c r="Q4" s="15"/>
       <c r="R4" s="72" t="s">
+        <v>242</v>
+      </c>
+      <c r="S4" s="72" t="s">
         <v>243</v>
       </c>
-      <c r="S4" s="72" t="s">
+      <c r="T4" s="72" t="s">
         <v>244</v>
-      </c>
-      <c r="T4" s="72" t="s">
-        <v>245</v>
       </c>
       <c r="U4" s="186"/>
       <c r="V4" s="73"/>
@@ -4474,8 +4489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4527,7 +4542,7 @@
         <v>161</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>134</v>
@@ -4536,13 +4551,13 @@
         <v>180</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>162</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="S2" s="9"/>
       <c r="T2" s="9"/>
@@ -4686,11 +4701,9 @@
       <c r="G4" s="175" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="101" t="s">
-        <v>157</v>
-      </c>
+      <c r="H4" s="101"/>
       <c r="I4" s="101" t="s">
-        <v>157</v>
+        <v>255</v>
       </c>
       <c r="J4" s="101" t="s">
         <v>157</v>
@@ -4781,7 +4794,7 @@
         <v>184</v>
       </c>
       <c r="F5" s="179" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G5" s="180" t="s">
         <v>185</v>
@@ -4946,7 +4959,7 @@
         <v>142</v>
       </c>
       <c r="F8" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H8" s="2">
         <v>49.2</v>
@@ -4966,7 +4979,7 @@
         <v>169</v>
       </c>
       <c r="F9" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H9" s="2">
         <v>48.1</v>
@@ -4986,7 +4999,7 @@
         <v>165</v>
       </c>
       <c r="F10" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H10" s="2">
         <v>46</v>
@@ -5006,12 +5019,12 @@
         <v>166</v>
       </c>
       <c r="F11" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H11" s="2">
         <v>49</v>
       </c>
-      <c r="I11" s="255">
+      <c r="I11" s="2">
         <v>0.3</v>
       </c>
       <c r="J11" s="155" t="s">
@@ -5026,12 +5039,12 @@
         <v>167</v>
       </c>
       <c r="F12" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H12" s="2">
         <v>41.3</v>
       </c>
-      <c r="I12" s="255">
+      <c r="I12" s="2">
         <v>0.3</v>
       </c>
       <c r="J12" s="154" t="s">
@@ -5046,12 +5059,12 @@
         <v>170</v>
       </c>
       <c r="F13" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H13" s="157">
         <v>41.66</v>
       </c>
-      <c r="I13" s="255">
+      <c r="I13" s="2">
         <v>0.3</v>
       </c>
       <c r="J13" s="2">
@@ -5066,7 +5079,7 @@
         <v>170</v>
       </c>
       <c r="F14" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H14" s="2">
         <v>45.4</v>
@@ -5086,12 +5099,12 @@
         <v>168</v>
       </c>
       <c r="F15" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H15" s="2">
         <v>46</v>
       </c>
-      <c r="I15" s="255" t="s">
+      <c r="I15" s="2" t="s">
         <v>160</v>
       </c>
       <c r="J15" s="2">
@@ -5103,15 +5116,15 @@
         <v>150</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F16" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H16" s="2">
         <v>40.799999999999997</v>
       </c>
-      <c r="I16" s="255">
+      <c r="I16" s="2">
         <v>0.3</v>
       </c>
       <c r="J16" s="2">
@@ -5126,12 +5139,12 @@
         <v>168</v>
       </c>
       <c r="F17" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H17" s="2">
         <v>41</v>
       </c>
-      <c r="I17" s="255">
+      <c r="I17" s="2">
         <v>0.3</v>
       </c>
       <c r="J17" s="2">
@@ -5146,12 +5159,12 @@
         <v>164</v>
       </c>
       <c r="F18" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H18" s="2">
         <v>41</v>
       </c>
-      <c r="I18" s="255">
+      <c r="I18" s="2">
         <v>0.3</v>
       </c>
       <c r="J18" s="2">
@@ -5166,12 +5179,12 @@
         <v>169</v>
       </c>
       <c r="F19" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H19" s="2">
         <v>37.700000000000003</v>
       </c>
-      <c r="I19" s="255">
+      <c r="I19" s="2">
         <v>0.3</v>
       </c>
       <c r="J19" s="2">
@@ -5186,12 +5199,12 @@
         <v>165</v>
       </c>
       <c r="F20" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H20" s="2">
         <v>41</v>
       </c>
-      <c r="I20" s="255">
+      <c r="I20" s="2">
         <v>0.3</v>
       </c>
       <c r="J20" s="2">
@@ -5206,12 +5219,12 @@
         <v>166</v>
       </c>
       <c r="F21" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H21" s="2">
         <v>39.5</v>
       </c>
-      <c r="I21" s="255">
+      <c r="I21" s="2">
         <v>0.3</v>
       </c>
       <c r="J21" s="2">
@@ -5226,12 +5239,12 @@
         <v>167</v>
       </c>
       <c r="F22" s="191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H22" s="2">
         <v>38.299999999999997</v>
       </c>
-      <c r="I22" s="255">
+      <c r="I22" s="2">
         <v>0.3</v>
       </c>
       <c r="J22" s="2">
@@ -5265,7 +5278,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5288,13 +5301,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="251" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="251"/>
-      <c r="C1" s="251"/>
-      <c r="D1" s="251"/>
-      <c r="E1" s="251"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
       <c r="F1" s="88" t="s">
         <v>25</v>
       </c>
@@ -5308,8 +5321,8 @@
       <c r="O1" s="22"/>
     </row>
     <row r="2" spans="1:15" s="21" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="245"/>
-      <c r="B2" s="246"/>
+      <c r="A2" s="246"/>
+      <c r="B2" s="247"/>
       <c r="C2" s="63"/>
       <c r="D2" s="64"/>
       <c r="E2" s="63"/>
@@ -5325,10 +5338,10 @@
       <c r="O2" s="22"/>
     </row>
     <row r="3" spans="1:15" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="247" t="s">
+      <c r="A3" s="248" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="248" t="s">
+      <c r="B3" s="249" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="20"/>
@@ -5457,7 +5470,7 @@
       <c r="B7" s="2"/>
       <c r="C7" s="56"/>
       <c r="D7" s="2" t="s">
-        <v>220</v>
+        <v>252</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -5475,17 +5488,23 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="104">
         <v>3</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="104">
         <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -5516,8 +5535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AF10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5585,8 +5604,8 @@
       <c r="AF1" s="22"/>
     </row>
     <row r="2" spans="1:32" s="21" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="245"/>
-      <c r="B2" s="246"/>
+      <c r="A2" s="246"/>
+      <c r="B2" s="247"/>
       <c r="C2" s="63"/>
       <c r="D2" s="64"/>
       <c r="E2" s="22"/>
@@ -5619,10 +5638,10 @@
       <c r="AF2" s="22"/>
     </row>
     <row r="3" spans="1:32" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="252" t="s">
+      <c r="A3" s="253" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="253" t="s">
+      <c r="B3" s="254" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="20"/>
@@ -5642,10 +5661,10 @@
       <c r="K3" s="86"/>
       <c r="L3" s="86"/>
       <c r="M3" s="20"/>
-      <c r="N3" s="249" t="s">
+      <c r="N3" s="250" t="s">
         <v>84</v>
       </c>
-      <c r="O3" s="249"/>
+      <c r="O3" s="250"/>
       <c r="P3" s="87"/>
       <c r="Q3" s="87"/>
       <c r="R3" s="20"/>

</xml_diff>